<commit_message>
updated spreadseets added stirling
</commit_message>
<xml_diff>
--- a/debate/ACM/states_ACM_regression_analysis.xlsx
+++ b/debate/ACM/states_ACM_regression_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stk\Documents\GitHub\covid\debate\ACM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C9DC3E-8D05-4892-A1E4-3FC3D8865F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8C5A6E-0F2E-4A4A-B0ED-063D46117784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="25140" windowHeight="13605" xr2:uid="{731BA8CD-4BE5-45C5-B932-9FB51EE0C43B}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3187" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3188" uniqueCount="167">
   <si>
     <t>State</t>
   </si>
@@ -541,12 +541,6 @@
     <t>r2</t>
   </si>
   <si>
-    <t>lower slope</t>
-  </si>
-  <si>
-    <t>upper slope</t>
-  </si>
-  <si>
     <t>Full</t>
   </si>
   <si>
@@ -563,6 +557,15 @@
   </si>
   <si>
     <t>Omit hawaii since no vax data</t>
+  </si>
+  <si>
+    <t>95% confidence intervals for the slope</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>high</t>
   </si>
 </sst>
 </file>
@@ -1151,7 +1154,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>21-22 monthly</a:t>
+              <a:t>21-22 average</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -1159,7 +1162,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>relative to 2020H2 basseline monthly ACM</a:t>
+              <a:t>relative to 2020H2 basseline  ACM</a:t>
             </a:r>
             <a:br>
               <a:rPr lang="en-US"/>
@@ -1170,7 +1173,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> level of the state</a:t>
+              <a:t> level of the state in doses per 100 people</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -13851,10 +13854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C517E209-A571-4121-A731-80892260C1EA}">
-  <dimension ref="A3:S58"/>
+  <dimension ref="A3:T58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8:N57"/>
+      <selection activeCell="AF32" sqref="AF32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13919,7 +13922,7 @@
         <v>88</v>
       </c>
       <c r="G4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H4" t="s">
         <v>89</v>
@@ -13961,7 +13964,7 @@
         <v>94</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="N7" s="4" t="s">
         <v>99</v>
@@ -15095,7 +15098,7 @@
         <v>5.826330165142516E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>59</v>
       </c>
@@ -15145,7 +15148,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>60</v>
       </c>
@@ -15195,7 +15198,7 @@
         <v>0.16294139132759816</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>61</v>
       </c>
@@ -15239,7 +15242,7 @@
         <v>1.024869731505724</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>62</v>
       </c>
@@ -15283,14 +15286,17 @@
         <v>1.0886032757051864</v>
       </c>
       <c r="Q36" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="R36">
         <f>R30-(2*R31)</f>
         <v>1.3166753824743521E-3</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T36" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>63</v>
       </c>
@@ -15334,14 +15340,14 @@
         <v>1.0971603563474388</v>
       </c>
       <c r="Q37" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="R37">
         <f>R30+(2*R31)</f>
         <v>3.2785337600128956E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>64</v>
       </c>
@@ -15385,7 +15391,7 @@
         <v>1.0163386480651055</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>65</v>
       </c>
@@ -15429,7 +15435,7 @@
         <v>1.1270389881949308</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>66</v>
       </c>
@@ -15473,7 +15479,7 @@
         <v>1.0364221059356404</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>67</v>
       </c>
@@ -15517,7 +15523,7 @@
         <v>0.81193816398801411</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>68</v>
       </c>
@@ -15561,7 +15567,7 @@
         <v>1.0054676639595679</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>69</v>
       </c>
@@ -15605,7 +15611,7 @@
         <v>1.0002689737740458</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>70</v>
       </c>
@@ -15649,7 +15655,7 @@
         <v>1.1100248800602672</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>71</v>
       </c>
@@ -15693,7 +15699,7 @@
         <v>1.0449683371185119</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>72</v>
       </c>
@@ -15737,7 +15743,7 @@
         <v>1.0443790924318563</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>73</v>
       </c>
@@ -15781,7 +15787,7 @@
         <v>0.97653065006300499</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>74</v>
       </c>
@@ -16261,7 +16267,7 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16277,7 +16283,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -43912,12 +43918,12 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
@@ -43927,7 +43933,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>